<commit_message>
Added 5 new data rows
</commit_message>
<xml_diff>
--- a/data/favrests.xlsx
+++ b/data/favrests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/p_hadjipakkos_1_research_gla_ac_uk/Documents/Documents/Github/NWB_demo/GitTutorial/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahwalters/Code/GitTutorial/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{8C525ED2-863F-46BE-B111-9757F683EF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CA14478-342C-4EBF-83B1-6718B1E8D728}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47391CCC-AC5C-3A42-BA01-ADA92C8DC63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1EA258AF-AAAE-42D4-987F-A8C59E6A05D3}"/>
+    <workbookView xWindow="12580" yWindow="7920" windowWidth="17660" windowHeight="10520" xr2:uid="{1EA258AF-AAAE-42D4-987F-A8C59E6A05D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>University</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>JMS</t>
+  </si>
+  <si>
+    <t>Amore</t>
+  </si>
+  <si>
+    <t>Curlers Rest</t>
   </si>
 </sst>
 </file>
@@ -437,19 +443,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F249C8-93BA-40B6-8A82-254138D982A1}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -465,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -473,7 +479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -481,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -489,7 +495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -497,7 +503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -505,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -513,7 +519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -521,7 +527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -529,12 +535,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>